<commit_message>
Added GSON to project & made some attempts to use it on meetings data.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Simple JSON parsing with gson.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>Tested API connection &amp; JSON parsing.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>3.5</v>
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +572,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Created layout for dynamic content. Backed up to layout_single_meeting_copy.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Tested API connection &amp; JSON parsing.</t>
+  </si>
+  <si>
+    <t>JSON parsing. Dynamic views for Meetings. V1.1 release.</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,6 +485,15 @@
       <c r="A6" s="2">
         <v>42281</v>
       </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1.7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -572,7 +584,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>5</v>
+        <v>6.7</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Done some video playback functionality.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +499,9 @@
       <c r="A7" s="2">
         <v>42282</v>
       </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -584,7 +587,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Renamed main_fragment. Changed agenda content viewing to webview.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>JSON parsing. Dynamic views for Meetings. V1.1 release.</t>
+  </si>
+  <si>
+    <t>Autoupdating agenda list.</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +510,12 @@
       <c r="A8" s="2">
         <v>42283</v>
       </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -587,7 +596,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Gradient backgrounds. Back to top buttons.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Autoupdating agenda list.</t>
+  </si>
+  <si>
+    <t>GUI layout.</t>
   </si>
 </sst>
 </file>
@@ -505,13 +508,16 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42283</v>
       </c>
       <c r="C8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -596,7 +602,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Small GUI update bug fixes.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -46,13 +46,31 @@
     <t>Tested API connection &amp; JSON parsing.</t>
   </si>
   <si>
-    <t>JSON parsing. Dynamic views for Meetings. V1.1 release.</t>
-  </si>
-  <si>
     <t>Autoupdating agenda list.</t>
   </si>
   <si>
     <t>GUI layout.</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>1.4a</t>
+  </si>
+  <si>
+    <t>JSON parsing. Dynamic views for Meetings.</t>
+  </si>
+  <si>
+    <t>Web view &amp; UI tweaks. Video button for testing.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2a</t>
+  </si>
+  <si>
+    <t>1.3a</t>
   </si>
 </sst>
 </file>
@@ -109,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -117,6 +135,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -422,20 +441,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +468,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42277</v>
       </c>
@@ -462,13 +485,15 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42278</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42279</v>
       </c>
@@ -481,13 +506,15 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42280</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42281</v>
       </c>
@@ -498,10 +525,16 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42282</v>
       </c>
@@ -509,10 +542,11 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42283</v>
       </c>
@@ -520,93 +554,125 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42284</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42285</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42286</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42287</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42288</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42289</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42290</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42291</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42292</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42293</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42294</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42295</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42296</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42297</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added menu item for helsinkikanava videos.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>1.3a</t>
+  </si>
+  <si>
+    <t>Bug fixes.</t>
   </si>
 </sst>
 </file>
@@ -443,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +593,12 @@
       <c r="A12" s="2">
         <v>42287</v>
       </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -664,7 +673,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Implemented fragment for agenda attachments.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Bug fixes.</t>
+  </si>
+  <si>
+    <t>New branch for old Helsinkikanava API.</t>
   </si>
 </sst>
 </file>
@@ -446,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +614,12 @@
       <c r="A14" s="2">
         <v>42289</v>
       </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,7 +682,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added file type to attachment header
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>New branch for old Helsinkikanava API.</t>
+  </si>
+  <si>
+    <t>1.5a</t>
+  </si>
+  <si>
+    <t>Attachments &amp; stability.</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +632,15 @@
       <c r="A15" s="2">
         <v>42290</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -682,7 +696,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>21.5</v>
+        <v>23.5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Implemented video data query. Play button starts meeting video.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +633,7 @@
         <v>42290</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -696,7 +696,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Created meetings view as first tab.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>1.6a</t>
+  </si>
+  <si>
+    <t>Fixed  serous bug with app crashing.</t>
+  </si>
+  <si>
+    <t>1,71a</t>
   </si>
 </sst>
 </file>
@@ -461,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +684,15 @@
       <c r="A19" s="2">
         <v>42294</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -710,7 +724,7 @@
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>26.5</v>
+        <v>30.5</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated app icon. Before updating package name to paatokset_helsinki.
</commit_message>
<xml_diff>
--- a/Documentation/WorkingHoursLog.xlsx
+++ b/Documentation/WorkingHoursLog.xlsx
@@ -31,9 +31,6 @@
     <t>Eetu</t>
   </si>
   <si>
-    <t>Deadline</t>
-  </si>
-  <si>
     <t>Project template &amp; exploring Android Studio.</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>1,71a</t>
+  </si>
+  <si>
+    <t>Major improvements in UI and logic. Twitter button and first release.</t>
   </si>
 </sst>
 </file>
@@ -467,15 +467,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5"/>
     </row>
@@ -528,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -549,13 +549,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5"/>
     </row>
@@ -578,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -598,10 +598,10 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -636,7 +636,7 @@
         <v>1.5</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -648,10 +648,10 @@
         <v>2.5</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>2.5</v>
       </c>
       <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,18 +688,21 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42295</v>
       </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
       <c r="D20" s="3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -720,14 +723,14 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <f>SUM(C2:C22)</f>
-        <v>30.5</v>
+        <v>39.5</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5"/>
     </row>

</xml_diff>